<commit_message>
non existing time solved
</commit_message>
<xml_diff>
--- a/Data/Regulatory_values.xlsx
+++ b/Data/Regulatory_values.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lolap\OneDrive\Documents\Cours\Master\Air pollution\AP\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheo\Desktop\EPFL\MA4\Air pollution\Air_pollution\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FCAF06-146C-46E5-929C-E2DF22A365FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F12E3E-9EC8-4829-A6A7-234C5AE4602A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
   <si>
     <t>Pollutants</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>Hourly mean [ug/m3]</t>
+  </si>
+  <si>
+    <t>SO2</t>
+  </si>
+  <si>
+    <t>CO</t>
   </si>
 </sst>
 </file>
@@ -372,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -456,6 +462,34 @@
         <v>7</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1">
+        <v>30</v>
+      </c>
+      <c r="C6">
+        <v>100</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1">
+        <v>8</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>